<commit_message>
Untraced Sum of Ar Amount updated
</commit_message>
<xml_diff>
--- a/OldMutual/Excel Template/StatementSummary.xlsx
+++ b/OldMutual/Excel Template/StatementSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91888\OneDrive\Documents\UiPath\Old Mutual Final - Ramesh\Old-Mutual-Excel-Automation\OldMutual\Excel Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB54DB8F-62DC-44FF-924E-5F0D31EF44CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C491D271-9769-4BA0-B647-02A54A1F11BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" xr2:uid="{574CCD08-F5A6-4833-9F7A-D19EC403FB22}"/>
   </bookViews>
@@ -685,7 +685,7 @@
   <cols>
     <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
     <col min="7" max="7" width="15.109375" customWidth="1"/>
     <col min="8" max="8" width="68.21875" customWidth="1"/>
   </cols>

</xml_diff>